<commit_message>
Updated stringsAsFactors in species list load for all examples
</commit_message>
<xml_diff>
--- a/examples/Test_DesignBased_Estimator/Design Based Estimates.xlsx
+++ b/examples/Test_DesignBased_Estimator/Design Based Estimates.xlsx
@@ -11,23 +11,22 @@
     <sheet name="GOA_Walleye pollock" r:id="rId5" sheetId="3"/>
     <sheet name="AI_Walleye pollock" r:id="rId6" sheetId="4"/>
     <sheet name="GOA_Pacific cod" r:id="rId7" sheetId="5"/>
-    <sheet name="EBS_SHELF_Pacific cod" r:id="rId8" sheetId="6"/>
-    <sheet name="AI_Pacific cod" r:id="rId9" sheetId="7"/>
-    <sheet name="GOA_Northern rockfish" r:id="rId10" sheetId="8"/>
-    <sheet name="AI_Northern rockfish" r:id="rId11" sheetId="9"/>
-    <sheet name="GOA_Dover sole" r:id="rId12" sheetId="10"/>
-    <sheet name="GOA_Big skate" r:id="rId13" sheetId="11"/>
-    <sheet name="AI_Atka mackerel" r:id="rId14" sheetId="12"/>
-    <sheet name="GOA_Harlequin rockfish" r:id="rId15" sheetId="13"/>
-    <sheet name="GOA_Arrowtooth flounder" r:id="rId16" sheetId="14"/>
-    <sheet name="EBS_SHELF_Arrowtooth flounder" r:id="rId17" sheetId="15"/>
-    <sheet name="GOA_Spiny dogfish" r:id="rId18" sheetId="16"/>
+    <sheet name="AI_Pacific cod" r:id="rId8" sheetId="6"/>
+    <sheet name="GOA_Northern rockfish" r:id="rId9" sheetId="7"/>
+    <sheet name="AI_Northern rockfish" r:id="rId10" sheetId="8"/>
+    <sheet name="GOA_Dover sole" r:id="rId11" sheetId="9"/>
+    <sheet name="GOA_Big skate" r:id="rId12" sheetId="10"/>
+    <sheet name="AI_Atka mackerel" r:id="rId13" sheetId="11"/>
+    <sheet name="GOA_Harlequin rockfish" r:id="rId14" sheetId="12"/>
+    <sheet name="GOA_Arrowtooth flounder" r:id="rId15" sheetId="13"/>
+    <sheet name="EBS_SHELF_Arrowtooth flounder" r:id="rId16" sheetId="14"/>
+    <sheet name="GOA_Spiny dogfish" r:id="rId17" sheetId="15"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="40">
   <si>
     <t>YEAR</t>
   </si>
@@ -534,16 +533,16 @@
         <v>1984.0</v>
       </c>
       <c r="C2" t="n">
-        <v>68633.7891577465</v>
+        <v>27607.26098099168</v>
       </c>
       <c r="D2" t="n">
-        <v>3.781212190838004E7</v>
+        <v>3.63870902418494E7</v>
       </c>
       <c r="E2" t="n">
-        <v>6149.156194827062</v>
+        <v>6032.171270931338</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08959371572351872</v>
+        <v>0.21849944748537878</v>
       </c>
     </row>
     <row r="3">
@@ -554,16 +553,16 @@
         <v>1987.0</v>
       </c>
       <c r="C3" t="n">
-        <v>63394.41607893733</v>
+        <v>28135.448866254927</v>
       </c>
       <c r="D3" t="n">
-        <v>5.458865352012821E7</v>
+        <v>1.9458763919439044E7</v>
       </c>
       <c r="E3" t="n">
-        <v>7388.413464345929</v>
+        <v>4411.208895466076</v>
       </c>
       <c r="F3" t="n">
-        <v>0.11654675476695045</v>
+        <v>0.15678473503071735</v>
       </c>
     </row>
     <row r="4">
@@ -574,16 +573,16 @@
         <v>1990.0</v>
       </c>
       <c r="C4" t="n">
-        <v>96596.8190505549</v>
+        <v>22316.209625023403</v>
       </c>
       <c r="D4" t="n">
-        <v>1.5313196731019202E8</v>
+        <v>3.1067899516477402E7</v>
       </c>
       <c r="E4" t="n">
-        <v>12374.650189407055</v>
+        <v>5573.8585841836175</v>
       </c>
       <c r="F4" t="n">
-        <v>0.12810618725375067</v>
+        <v>0.24976726235505473</v>
       </c>
     </row>
     <row r="5">
@@ -594,16 +593,16 @@
         <v>1993.0</v>
       </c>
       <c r="C5" t="n">
-        <v>85549.05085398392</v>
+        <v>39707.88591302294</v>
       </c>
       <c r="D5" t="n">
-        <v>4.148786820351742E7</v>
+        <v>5.0551143753639035E7</v>
       </c>
       <c r="E5" t="n">
-        <v>6441.107684514941</v>
+        <v>7109.932753102454</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0752913985627812</v>
+        <v>0.1790559378727997</v>
       </c>
     </row>
     <row r="6">
@@ -614,16 +613,16 @@
         <v>1996.0</v>
       </c>
       <c r="C6" t="n">
-        <v>79530.24950163432</v>
+        <v>43063.85711407673</v>
       </c>
       <c r="D6" t="n">
-        <v>3.1628340545021616E7</v>
+        <v>5.7619096019248925E7</v>
       </c>
       <c r="E6" t="n">
-        <v>5623.907942438391</v>
+        <v>7590.724340881371</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07071407392381966</v>
+        <v>0.176266708315826</v>
       </c>
     </row>
     <row r="7">
@@ -634,16 +633,16 @@
         <v>1999.0</v>
       </c>
       <c r="C7" t="n">
-        <v>74245.21680594703</v>
+        <v>54650.40122964112</v>
       </c>
       <c r="D7" t="n">
-        <v>2.7413205957390133E7</v>
+        <v>6.473976859722426E7</v>
       </c>
       <c r="E7" t="n">
-        <v>5235.762213602728</v>
+        <v>8046.102696164415</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07051985890602644</v>
+        <v>0.14722861159526848</v>
       </c>
     </row>
     <row r="8">
@@ -654,16 +653,16 @@
         <v>2001.0</v>
       </c>
       <c r="C8" t="n">
-        <v>32423.90797904045</v>
+        <v>39082.269256227046</v>
       </c>
       <c r="D8" t="n">
-        <v>1.4122295718716972E7</v>
+        <v>5.3147045221041895E7</v>
       </c>
       <c r="E8" t="n">
-        <v>3757.9643051414114</v>
+        <v>7290.202001388021</v>
       </c>
       <c r="F8" t="n">
-        <v>0.11590102919027048</v>
+        <v>0.1865347673031156</v>
       </c>
     </row>
     <row r="9">
@@ -674,16 +673,16 @@
         <v>2003.0</v>
       </c>
       <c r="C9" t="n">
-        <v>99296.62617433087</v>
+        <v>55396.712638026154</v>
       </c>
       <c r="D9" t="n">
-        <v>1.1118576120922644E8</v>
+        <v>8.238689065300226E7</v>
       </c>
       <c r="E9" t="n">
-        <v>10544.46590440817</v>
+        <v>9076.722462045553</v>
       </c>
       <c r="F9" t="n">
-        <v>0.10619158284286215</v>
+        <v>0.1638494782416924</v>
       </c>
     </row>
     <row r="10">
@@ -694,16 +693,16 @@
         <v>2005.0</v>
       </c>
       <c r="C10" t="n">
-        <v>80560.47717498823</v>
+        <v>39319.86281069215</v>
       </c>
       <c r="D10" t="n">
-        <v>4.620545637460832E7</v>
+        <v>4.034092227196407E7</v>
       </c>
       <c r="E10" t="n">
-        <v>6797.459552995392</v>
+        <v>6351.450406951476</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08437710141947635</v>
+        <v>0.16153287302987085</v>
       </c>
     </row>
     <row r="11">
@@ -714,16 +713,16 @@
         <v>2007.0</v>
       </c>
       <c r="C11" t="n">
-        <v>71468.5091960996</v>
+        <v>39629.54527380366</v>
       </c>
       <c r="D11" t="n">
-        <v>5.056779960558433E7</v>
+        <v>5.9199359614076205E7</v>
       </c>
       <c r="E11" t="n">
-        <v>7111.103965319613</v>
+        <v>7694.112009457375</v>
       </c>
       <c r="F11" t="n">
-        <v>0.09949982230366296</v>
+        <v>0.1941509032288447</v>
       </c>
     </row>
     <row r="12">
@@ -734,16 +733,16 @@
         <v>2009.0</v>
       </c>
       <c r="C12" t="n">
-        <v>76276.93110273265</v>
+        <v>44349.291792831245</v>
       </c>
       <c r="D12" t="n">
-        <v>4.1433952986025654E7</v>
+        <v>5.118320302631646E7</v>
       </c>
       <c r="E12" t="n">
-        <v>6436.9210796797615</v>
+        <v>7154.243707500916</v>
       </c>
       <c r="F12" t="n">
-        <v>0.08438883141496967</v>
+        <v>0.1613158501136956</v>
       </c>
     </row>
     <row r="13">
@@ -754,16 +753,16 @@
         <v>2011.0</v>
       </c>
       <c r="C13" t="n">
-        <v>77530.87007075697</v>
+        <v>67882.7439925255</v>
       </c>
       <c r="D13" t="n">
-        <v>5.472765854450502E7</v>
+        <v>6.181668838650324E8</v>
       </c>
       <c r="E13" t="n">
-        <v>7397.814443773582</v>
+        <v>24862.962089522487</v>
       </c>
       <c r="F13" t="n">
-        <v>0.09541766314530092</v>
+        <v>0.36626336278127064</v>
       </c>
     </row>
     <row r="14">
@@ -774,16 +773,16 @@
         <v>2013.0</v>
       </c>
       <c r="C14" t="n">
-        <v>82738.89311549942</v>
+        <v>38233.60674072062</v>
       </c>
       <c r="D14" t="n">
-        <v>3.200149172776994E8</v>
+        <v>9.57496800278743E7</v>
       </c>
       <c r="E14" t="n">
-        <v>17888.960765726428</v>
+        <v>9785.176545564946</v>
       </c>
       <c r="F14" t="n">
-        <v>0.21620981490233765</v>
+        <v>0.2559312965664645</v>
       </c>
     </row>
     <row r="15">
@@ -794,16 +793,16 @@
         <v>2015.0</v>
       </c>
       <c r="C15" t="n">
-        <v>53067.00075185715</v>
+        <v>58005.59006429978</v>
       </c>
       <c r="D15" t="n">
-        <v>2.4956950153002646E7</v>
+        <v>9.766696315547307E7</v>
       </c>
       <c r="E15" t="n">
-        <v>4995.693160413542</v>
+        <v>9882.659720716538</v>
       </c>
       <c r="F15" t="n">
-        <v>0.09413935382882385</v>
+        <v>0.17037426409698633</v>
       </c>
     </row>
   </sheetData>
@@ -842,19 +841,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1984.0</v>
+        <v>1980.0</v>
       </c>
       <c r="C2" t="n">
-        <v>27607.26098099168</v>
+        <v>96046.22343414213</v>
       </c>
       <c r="D2" t="n">
-        <v>3.63870902418494E7</v>
+        <v>3.100537997472533E9</v>
       </c>
       <c r="E2" t="n">
-        <v>6032.171270931338</v>
+        <v>55682.47477862791</v>
       </c>
       <c r="F2" t="n">
-        <v>0.21849944748537878</v>
+        <v>0.5797466343568292</v>
       </c>
     </row>
     <row r="3">
@@ -862,19 +861,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1987.0</v>
+        <v>1983.0</v>
       </c>
       <c r="C3" t="n">
-        <v>28135.448866254927</v>
+        <v>489328.247886811</v>
       </c>
       <c r="D3" t="n">
-        <v>1.9458763919439044E7</v>
+        <v>1.4251922185486778E10</v>
       </c>
       <c r="E3" t="n">
-        <v>4411.208895466076</v>
+        <v>119381.41474068222</v>
       </c>
       <c r="F3" t="n">
-        <v>0.15678473503071735</v>
+        <v>0.24397000429923463</v>
       </c>
     </row>
     <row r="4">
@@ -882,19 +881,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1990.0</v>
+        <v>1986.0</v>
       </c>
       <c r="C4" t="n">
-        <v>22316.209625023403</v>
+        <v>1119578.1102116606</v>
       </c>
       <c r="D4" t="n">
-        <v>3.1067899516477402E7</v>
+        <v>8.064996720495623E11</v>
       </c>
       <c r="E4" t="n">
-        <v>5573.8585841836175</v>
+        <v>898053.2679354617</v>
       </c>
       <c r="F4" t="n">
-        <v>0.24976726235505473</v>
+        <v>0.8021354291802661</v>
       </c>
     </row>
     <row r="5">
@@ -902,19 +901,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1993.0</v>
+        <v>1991.0</v>
       </c>
       <c r="C5" t="n">
-        <v>39707.88591302294</v>
+        <v>708298.7534878738</v>
       </c>
       <c r="D5" t="n">
-        <v>5.0551143753639035E7</v>
+        <v>1.0470463010159054E10</v>
       </c>
       <c r="E5" t="n">
-        <v>7109.932753102454</v>
+        <v>102325.28040596348</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1790559378727997</v>
+        <v>0.14446627203857604</v>
       </c>
     </row>
     <row r="6">
@@ -922,19 +921,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1996.0</v>
+        <v>1994.0</v>
       </c>
       <c r="C6" t="n">
-        <v>43063.85711407673</v>
+        <v>686007.1910861329</v>
       </c>
       <c r="D6" t="n">
-        <v>5.7619096019248925E7</v>
+        <v>4.943568881471019E10</v>
       </c>
       <c r="E6" t="n">
-        <v>7590.724340881371</v>
+        <v>222341.37899795035</v>
       </c>
       <c r="F6" t="n">
-        <v>0.176266708315826</v>
+        <v>0.3241093998532646</v>
       </c>
     </row>
     <row r="7">
@@ -942,19 +941,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1999.0</v>
+        <v>1997.0</v>
       </c>
       <c r="C7" t="n">
-        <v>54650.40122964112</v>
+        <v>461997.08226931136</v>
       </c>
       <c r="D7" t="n">
-        <v>6.473976859722426E7</v>
+        <v>2.0057614775514145E10</v>
       </c>
       <c r="E7" t="n">
-        <v>8046.102696164415</v>
+        <v>141624.90873964984</v>
       </c>
       <c r="F7" t="n">
-        <v>0.14722861159526848</v>
+        <v>0.3065493575067485</v>
       </c>
     </row>
     <row r="8">
@@ -962,19 +961,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2001.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C8" t="n">
-        <v>39082.269256227046</v>
+        <v>512896.8249749221</v>
       </c>
       <c r="D8" t="n">
-        <v>5.3147045221041895E7</v>
+        <v>2.096479969970902E10</v>
       </c>
       <c r="E8" t="n">
-        <v>7290.202001388021</v>
+        <v>144792.26394980162</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1865347673031156</v>
+        <v>0.2823029055734186</v>
       </c>
     </row>
     <row r="9">
@@ -982,19 +981,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2003.0</v>
+        <v>2002.0</v>
       </c>
       <c r="C9" t="n">
-        <v>55396.712638026154</v>
+        <v>836194.9252381887</v>
       </c>
       <c r="D9" t="n">
-        <v>8.238689065300226E7</v>
+        <v>2.824343047964828E10</v>
       </c>
       <c r="E9" t="n">
-        <v>9076.722462045553</v>
+        <v>168057.81885901137</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1638494782416924</v>
+        <v>0.2009792379583509</v>
       </c>
     </row>
     <row r="10">
@@ -1002,19 +1001,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2005.0</v>
+        <v>2004.0</v>
       </c>
       <c r="C10" t="n">
-        <v>39319.86281069215</v>
+        <v>1157083.8697826166</v>
       </c>
       <c r="D10" t="n">
-        <v>4.034092227196407E7</v>
+        <v>3.6547193927406136E10</v>
       </c>
       <c r="E10" t="n">
-        <v>6351.450406951476</v>
+        <v>191173.20399942598</v>
       </c>
       <c r="F10" t="n">
-        <v>0.16153287302987085</v>
+        <v>0.16521983323070785</v>
       </c>
     </row>
     <row r="11">
@@ -1022,19 +1021,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2007.0</v>
+        <v>2006.0</v>
       </c>
       <c r="C11" t="n">
-        <v>39629.54527380366</v>
+        <v>741648.47638534</v>
       </c>
       <c r="D11" t="n">
-        <v>5.9199359614076205E7</v>
+        <v>4.225438100701579E10</v>
       </c>
       <c r="E11" t="n">
-        <v>7694.112009457375</v>
+        <v>205558.70452747992</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1941509032288447</v>
+        <v>0.27716460165783086</v>
       </c>
     </row>
     <row r="12">
@@ -1042,19 +1041,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2009.0</v>
+        <v>2010.0</v>
       </c>
       <c r="C12" t="n">
-        <v>44349.291792831245</v>
+        <v>930251.3348103752</v>
       </c>
       <c r="D12" t="n">
-        <v>5.118320302631646E7</v>
+        <v>1.0816679383403786E11</v>
       </c>
       <c r="E12" t="n">
-        <v>7154.243707500916</v>
+        <v>328887.2053364768</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1613158501136956</v>
+        <v>0.35354660942627725</v>
       </c>
     </row>
     <row r="13">
@@ -1062,19 +1061,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2011.0</v>
+        <v>2012.0</v>
       </c>
       <c r="C13" t="n">
-        <v>67882.7439925255</v>
+        <v>276876.2175119125</v>
       </c>
       <c r="D13" t="n">
-        <v>6.181668838650324E8</v>
+        <v>2.5013975740895233E9</v>
       </c>
       <c r="E13" t="n">
-        <v>24862.962089522487</v>
+        <v>50013.97378822766</v>
       </c>
       <c r="F13" t="n">
-        <v>0.36626336278127064</v>
+        <v>0.18063658279381045</v>
       </c>
     </row>
     <row r="14">
@@ -1082,19 +1081,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2013.0</v>
+        <v>2014.0</v>
       </c>
       <c r="C14" t="n">
-        <v>38233.60674072062</v>
+        <v>723927.573270405</v>
       </c>
       <c r="D14" t="n">
-        <v>9.57496800278743E7</v>
+        <v>3.097458850823993E10</v>
       </c>
       <c r="E14" t="n">
-        <v>9785.176545564946</v>
+        <v>175995.99003454574</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2559312965664645</v>
+        <v>0.24311270427160103</v>
       </c>
     </row>
     <row r="15">
@@ -1102,19 +1101,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2015.0</v>
+        <v>2016.0</v>
       </c>
       <c r="C15" t="n">
-        <v>58005.59006429978</v>
+        <v>448165.610178224</v>
       </c>
       <c r="D15" t="n">
-        <v>9.766696315547307E7</v>
+        <v>1.9169404206104855E10</v>
       </c>
       <c r="E15" t="n">
-        <v>9882.659720716538</v>
+        <v>138453.61752624906</v>
       </c>
       <c r="F15" t="n">
-        <v>0.17037426409698633</v>
+        <v>0.30893405112273026</v>
       </c>
     </row>
   </sheetData>
@@ -1153,19 +1152,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1980.0</v>
+        <v>1984.0</v>
       </c>
       <c r="C2" t="n">
-        <v>96046.22343414213</v>
+        <v>2626.389691987402</v>
       </c>
       <c r="D2" t="n">
-        <v>3.100537997472533E9</v>
+        <v>682860.1566988972</v>
       </c>
       <c r="E2" t="n">
-        <v>55682.47477862791</v>
+        <v>826.3535300940496</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5797466343568292</v>
+        <v>0.3146347751116643</v>
       </c>
     </row>
     <row r="3">
@@ -1173,19 +1172,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1983.0</v>
+        <v>1987.0</v>
       </c>
       <c r="C3" t="n">
-        <v>489328.247886811</v>
+        <v>72442.38055867594</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4251922185486778E10</v>
+        <v>4.529916182987597E8</v>
       </c>
       <c r="E3" t="n">
-        <v>119381.41474068222</v>
+        <v>21283.5997495433</v>
       </c>
       <c r="F3" t="n">
-        <v>0.24397000429923463</v>
+        <v>0.2938003912268494</v>
       </c>
     </row>
     <row r="4">
@@ -1193,19 +1192,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1986.0</v>
+        <v>1990.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1119578.1102116606</v>
+        <v>17664.16611885209</v>
       </c>
       <c r="D4" t="n">
-        <v>8.064996720495623E11</v>
+        <v>8.09229333554034E7</v>
       </c>
       <c r="E4" t="n">
-        <v>898053.2679354617</v>
+        <v>8995.71750086692</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8021354291802661</v>
+        <v>0.5092636380534395</v>
       </c>
     </row>
     <row r="5">
@@ -1213,19 +1212,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1991.0</v>
+        <v>1993.0</v>
       </c>
       <c r="C5" t="n">
-        <v>708298.7534878738</v>
+        <v>9280.331816088936</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0470463010159054E10</v>
+        <v>1.92803175129331E7</v>
       </c>
       <c r="E5" t="n">
-        <v>102325.28040596348</v>
+        <v>4390.935835665684</v>
       </c>
       <c r="F5" t="n">
-        <v>0.14446627203857604</v>
+        <v>0.4731442714206938</v>
       </c>
     </row>
     <row r="6">
@@ -1233,19 +1232,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1994.0</v>
+        <v>1996.0</v>
       </c>
       <c r="C6" t="n">
-        <v>686007.1910861329</v>
+        <v>20026.180696345502</v>
       </c>
       <c r="D6" t="n">
-        <v>4.943568881471019E10</v>
+        <v>1.6449094043000484E8</v>
       </c>
       <c r="E6" t="n">
-        <v>222341.37899795035</v>
+        <v>12825.402154708634</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3241093998532646</v>
+        <v>0.6404317602631584</v>
       </c>
     </row>
     <row r="7">
@@ -1253,19 +1252,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1997.0</v>
+        <v>1999.0</v>
       </c>
       <c r="C7" t="n">
-        <v>461997.08226931136</v>
+        <v>9876.455798164</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0057614775514145E10</v>
+        <v>1.7587023729982942E7</v>
       </c>
       <c r="E7" t="n">
-        <v>141624.90873964984</v>
+        <v>4193.68855901138</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3065493575067485</v>
+        <v>0.4246147246253026</v>
       </c>
     </row>
     <row r="8">
@@ -1273,19 +1272,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2000.0</v>
+        <v>2001.0</v>
       </c>
       <c r="C8" t="n">
-        <v>512896.8249749221</v>
+        <v>8364.758885037541</v>
       </c>
       <c r="D8" t="n">
-        <v>2.096479969970902E10</v>
+        <v>1.7384056647100657E7</v>
       </c>
       <c r="E8" t="n">
-        <v>144792.26394980162</v>
+        <v>4169.419221798242</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2823029055734186</v>
+        <v>0.4984506163418875</v>
       </c>
     </row>
     <row r="9">
@@ -1293,19 +1292,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2002.0</v>
+        <v>2003.0</v>
       </c>
       <c r="C9" t="n">
-        <v>836194.9252381887</v>
+        <v>3544.5060077191006</v>
       </c>
       <c r="D9" t="n">
-        <v>2.824343047964828E10</v>
+        <v>2504457.859749455</v>
       </c>
       <c r="E9" t="n">
-        <v>168057.81885901137</v>
+        <v>1582.5479012495814</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2009792379583509</v>
+        <v>0.44647911381816374</v>
       </c>
     </row>
     <row r="10">
@@ -1313,19 +1312,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2004.0</v>
+        <v>2005.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1157083.8697826166</v>
+        <v>33123.830545008124</v>
       </c>
       <c r="D10" t="n">
-        <v>3.6547193927406136E10</v>
+        <v>4.5482684441757476E8</v>
       </c>
       <c r="E10" t="n">
-        <v>191173.20399942598</v>
+        <v>21326.669792013352</v>
       </c>
       <c r="F10" t="n">
-        <v>0.16521983323070785</v>
+        <v>0.6438467242801227</v>
       </c>
     </row>
     <row r="11">
@@ -1333,19 +1332,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2006.0</v>
+        <v>2007.0</v>
       </c>
       <c r="C11" t="n">
-        <v>741648.47638534</v>
+        <v>4057.039664395374</v>
       </c>
       <c r="D11" t="n">
-        <v>4.225438100701579E10</v>
+        <v>3373252.395738241</v>
       </c>
       <c r="E11" t="n">
-        <v>205558.70452747992</v>
+        <v>1836.6416078642671</v>
       </c>
       <c r="F11" t="n">
-        <v>0.27716460165783086</v>
+        <v>0.4527048685233853</v>
       </c>
     </row>
     <row r="12">
@@ -1353,19 +1352,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2010.0</v>
+        <v>2009.0</v>
       </c>
       <c r="C12" t="n">
-        <v>930251.3348103752</v>
+        <v>2686.073583699452</v>
       </c>
       <c r="D12" t="n">
-        <v>1.0816679383403786E11</v>
+        <v>1328628.8173469931</v>
       </c>
       <c r="E12" t="n">
-        <v>328887.2053364768</v>
+        <v>1152.6616230910931</v>
       </c>
       <c r="F12" t="n">
-        <v>0.35354660942627725</v>
+        <v>0.4291251103789813</v>
       </c>
     </row>
     <row r="13">
@@ -1373,19 +1372,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2012.0</v>
+        <v>2011.0</v>
       </c>
       <c r="C13" t="n">
-        <v>276876.2175119125</v>
+        <v>3734.52297336727</v>
       </c>
       <c r="D13" t="n">
-        <v>2.5013975740895233E9</v>
+        <v>5241254.955368459</v>
       </c>
       <c r="E13" t="n">
-        <v>50013.97378822766</v>
+        <v>2289.378726940665</v>
       </c>
       <c r="F13" t="n">
-        <v>0.18063658279381045</v>
+        <v>0.6130311001612138</v>
       </c>
     </row>
     <row r="14">
@@ -1393,19 +1392,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2014.0</v>
+        <v>2013.0</v>
       </c>
       <c r="C14" t="n">
-        <v>723927.573270405</v>
+        <v>7485.280399424959</v>
       </c>
       <c r="D14" t="n">
-        <v>3.097458850823993E10</v>
+        <v>2.813682137519677E7</v>
       </c>
       <c r="E14" t="n">
-        <v>175995.99003454574</v>
+        <v>5304.415271752087</v>
       </c>
       <c r="F14" t="n">
-        <v>0.24311270427160103</v>
+        <v>0.7086461680392879</v>
       </c>
     </row>
     <row r="15">
@@ -1413,19 +1412,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2016.0</v>
+        <v>2015.0</v>
       </c>
       <c r="C15" t="n">
-        <v>448165.610178224</v>
+        <v>2316.3737919079676</v>
       </c>
       <c r="D15" t="n">
-        <v>1.9169404206104855E10</v>
+        <v>1214862.6850282152</v>
       </c>
       <c r="E15" t="n">
-        <v>138453.61752624906</v>
+        <v>1102.2080951563617</v>
       </c>
       <c r="F15" t="n">
-        <v>0.30893405112273026</v>
+        <v>0.47583343370867914</v>
       </c>
     </row>
   </sheetData>
@@ -1467,16 +1466,16 @@
         <v>1984.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2626.389691987402</v>
+        <v>1113688.2366634742</v>
       </c>
       <c r="D2" t="n">
-        <v>682860.1566988972</v>
+        <v>5.271037700006614E9</v>
       </c>
       <c r="E2" t="n">
-        <v>826.3535300940496</v>
+        <v>72601.9125092901</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3146347751116643</v>
+        <v>0.06519051752472481</v>
       </c>
     </row>
     <row r="3">
@@ -1487,16 +1486,16 @@
         <v>1987.0</v>
       </c>
       <c r="C3" t="n">
-        <v>72442.38055867594</v>
+        <v>932527.5986748552</v>
       </c>
       <c r="D3" t="n">
-        <v>4.529916182987597E8</v>
+        <v>5.477530649940076E9</v>
       </c>
       <c r="E3" t="n">
-        <v>21283.5997495433</v>
+        <v>74010.34150671159</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2938003912268494</v>
+        <v>0.07936530952207968</v>
       </c>
     </row>
     <row r="4">
@@ -1507,16 +1506,16 @@
         <v>1990.0</v>
       </c>
       <c r="C4" t="n">
-        <v>17664.16611885209</v>
+        <v>1907176.4078061914</v>
       </c>
       <c r="D4" t="n">
-        <v>8.09229333554034E7</v>
+        <v>5.968620909823026E10</v>
       </c>
       <c r="E4" t="n">
-        <v>8995.71750086692</v>
+        <v>244307.61162565168</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5092636380534395</v>
+        <v>0.12809911585823183</v>
       </c>
     </row>
     <row r="5">
@@ -1527,16 +1526,16 @@
         <v>1993.0</v>
       </c>
       <c r="C5" t="n">
-        <v>9280.331816088936</v>
+        <v>1551656.8743111603</v>
       </c>
       <c r="D5" t="n">
-        <v>1.92803175129331E7</v>
+        <v>1.0021763081454073E10</v>
       </c>
       <c r="E5" t="n">
-        <v>4390.935835665684</v>
+        <v>100108.7562676416</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4731442714206938</v>
+        <v>0.0645173284925404</v>
       </c>
     </row>
     <row r="6">
@@ -1547,16 +1546,16 @@
         <v>1996.0</v>
       </c>
       <c r="C6" t="n">
-        <v>20026.180696345502</v>
+        <v>1639631.8565418106</v>
       </c>
       <c r="D6" t="n">
-        <v>1.6449094043000484E8</v>
+        <v>1.314061298067534E10</v>
       </c>
       <c r="E6" t="n">
-        <v>12825.402154708634</v>
+        <v>114632.51275565471</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6404317602631584</v>
+        <v>0.06991356766965304</v>
       </c>
     </row>
     <row r="7">
@@ -1567,16 +1566,16 @@
         <v>1999.0</v>
       </c>
       <c r="C7" t="n">
-        <v>9876.455798164</v>
+        <v>1262150.7668057687</v>
       </c>
       <c r="D7" t="n">
-        <v>1.7587023729982942E7</v>
+        <v>9.86272475434545E9</v>
       </c>
       <c r="E7" t="n">
-        <v>4193.68855901138</v>
+        <v>99311.25190201486</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4246147246253026</v>
+        <v>0.07868414337959816</v>
       </c>
     </row>
     <row r="8">
@@ -1587,16 +1586,16 @@
         <v>2001.0</v>
       </c>
       <c r="C8" t="n">
-        <v>8364.758885037541</v>
+        <v>1360737.9511147256</v>
       </c>
       <c r="D8" t="n">
-        <v>1.7384056647100657E7</v>
+        <v>2.3012755190305473E10</v>
       </c>
       <c r="E8" t="n">
-        <v>4169.419221798242</v>
+        <v>151699.5556694398</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4984506163418875</v>
+        <v>0.1114832988564525</v>
       </c>
     </row>
     <row r="9">
@@ -1607,16 +1606,16 @@
         <v>2003.0</v>
       </c>
       <c r="C9" t="n">
-        <v>3544.5060077191006</v>
+        <v>2819095.0589319686</v>
       </c>
       <c r="D9" t="n">
-        <v>2504457.859749455</v>
+        <v>1.3738256480672762E11</v>
       </c>
       <c r="E9" t="n">
-        <v>1582.5479012495814</v>
+        <v>370651.5409474614</v>
       </c>
       <c r="F9" t="n">
-        <v>0.44647911381816374</v>
+        <v>0.13147890837277584</v>
       </c>
     </row>
     <row r="10">
@@ -1627,16 +1626,16 @@
         <v>2005.0</v>
       </c>
       <c r="C10" t="n">
-        <v>33123.830545008124</v>
+        <v>1899587.2172002746</v>
       </c>
       <c r="D10" t="n">
-        <v>4.5482684441757476E8</v>
+        <v>1.5826192714307724E10</v>
       </c>
       <c r="E10" t="n">
-        <v>21326.669792013352</v>
+        <v>125802.19677854487</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6438467242801227</v>
+        <v>0.06622607040068404</v>
       </c>
     </row>
     <row r="11">
@@ -1647,16 +1646,16 @@
         <v>2007.0</v>
       </c>
       <c r="C11" t="n">
-        <v>4057.039664395374</v>
+        <v>1936020.0922576024</v>
       </c>
       <c r="D11" t="n">
-        <v>3373252.395738241</v>
+        <v>2.2525944700190365E10</v>
       </c>
       <c r="E11" t="n">
-        <v>1836.6416078642671</v>
+        <v>150086.45741768432</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4527048685233853</v>
+        <v>0.07752319204635308</v>
       </c>
     </row>
     <row r="12">
@@ -1667,16 +1666,16 @@
         <v>2009.0</v>
       </c>
       <c r="C12" t="n">
-        <v>2686.073583699452</v>
+        <v>1772029.3527047152</v>
       </c>
       <c r="D12" t="n">
-        <v>1328628.8173469931</v>
+        <v>2.5409008475328747E10</v>
       </c>
       <c r="E12" t="n">
-        <v>1152.6616230910931</v>
+        <v>159402.03410034877</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4291251103789813</v>
+        <v>0.08995451111294936</v>
       </c>
     </row>
     <row r="13">
@@ -1687,16 +1686,16 @@
         <v>2011.0</v>
       </c>
       <c r="C13" t="n">
-        <v>3734.52297336727</v>
+        <v>1747338.8200396465</v>
       </c>
       <c r="D13" t="n">
-        <v>5241254.955368459</v>
+        <v>3.2328164491159664E10</v>
       </c>
       <c r="E13" t="n">
-        <v>2289.378726940665</v>
+        <v>179800.34619310292</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6130311001612138</v>
+        <v>0.1028995316369285</v>
       </c>
     </row>
     <row r="14">
@@ -1707,16 +1706,16 @@
         <v>2013.0</v>
       </c>
       <c r="C14" t="n">
-        <v>7485.280399424959</v>
+        <v>1290727.177071432</v>
       </c>
       <c r="D14" t="n">
-        <v>2.813682137519677E7</v>
+        <v>1.6990783870255583E10</v>
       </c>
       <c r="E14" t="n">
-        <v>5304.415271752087</v>
+        <v>130348.70106853993</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7086461680392879</v>
+        <v>0.1009885771246344</v>
       </c>
     </row>
     <row r="15">
@@ -1727,16 +1726,16 @@
         <v>2015.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2316.3737919079676</v>
+        <v>1659129.0751294277</v>
       </c>
       <c r="D15" t="n">
-        <v>1214862.6850282152</v>
+        <v>1.795212894694677E10</v>
       </c>
       <c r="E15" t="n">
-        <v>1102.2080951563617</v>
+        <v>133985.55499361403</v>
       </c>
       <c r="F15" t="n">
-        <v>0.47583343370867914</v>
+        <v>0.08075655896944721</v>
       </c>
     </row>
   </sheetData>
@@ -1775,19 +1774,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1984.0</v>
+        <v>1982.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1113688.2366634742</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>5.271037700006614E9</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n">
-        <v>72601.9125092901</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.06519051752472481</v>
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3">
@@ -1795,19 +1794,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1987.0</v>
+        <v>1983.0</v>
       </c>
       <c r="C3" t="n">
-        <v>932527.5986748552</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>5.477530649940076E9</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>74010.34150671159</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.07936530952207968</v>
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4">
@@ -1815,19 +1814,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1990.0</v>
+        <v>1984.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1907176.4078061914</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.968620909823026E10</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>244307.61162565168</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.12809911585823183</v>
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5">
@@ -1835,19 +1834,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1993.0</v>
+        <v>1985.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1551656.8743111603</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0021763081454073E10</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>100108.7562676416</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.0645173284925404</v>
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6">
@@ -1855,19 +1854,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1996.0</v>
+        <v>1986.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1639631.8565418106</v>
+        <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.314061298067534E10</v>
+        <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>114632.51275565471</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.06991356766965304</v>
+        <v>0.0</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7">
@@ -1875,19 +1874,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1999.0</v>
+        <v>1987.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1262150.7668057687</v>
+        <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>9.86272475434545E9</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>99311.25190201486</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.07868414337959816</v>
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8">
@@ -1895,19 +1894,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2001.0</v>
+        <v>1988.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1360737.9511147256</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2.3012755190305473E10</v>
+        <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>151699.5556694398</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1114832988564525</v>
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9">
@@ -1915,19 +1914,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2003.0</v>
+        <v>1989.0</v>
       </c>
       <c r="C9" t="n">
-        <v>2819095.0589319686</v>
+        <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.3738256480672762E11</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="n">
-        <v>370651.5409474614</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.13147890837277584</v>
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10">
@@ -1935,19 +1934,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2005.0</v>
+        <v>1990.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1899587.2172002746</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.5826192714307724E10</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n">
-        <v>125802.19677854487</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.06622607040068404</v>
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11">
@@ -1955,19 +1954,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2007.0</v>
+        <v>1991.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1936020.0922576024</v>
+        <v>0.0</v>
       </c>
       <c r="D11" t="n">
-        <v>2.2525944700190365E10</v>
+        <v>0.0</v>
       </c>
       <c r="E11" t="n">
-        <v>150086.45741768432</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.07752319204635308</v>
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12">
@@ -1975,19 +1974,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2009.0</v>
+        <v>1992.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1772029.3527047152</v>
+        <v>0.0</v>
       </c>
       <c r="D12" t="n">
-        <v>2.5409008475328747E10</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="n">
-        <v>159402.03410034877</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.08995451111294936</v>
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13">
@@ -1995,19 +1994,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2011.0</v>
+        <v>1993.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1747338.8200396465</v>
+        <v>0.0</v>
       </c>
       <c r="D13" t="n">
-        <v>3.2328164491159664E10</v>
+        <v>0.0</v>
       </c>
       <c r="E13" t="n">
-        <v>179800.34619310292</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.1028995316369285</v>
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14">
@@ -2015,19 +2014,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2013.0</v>
+        <v>1994.0</v>
       </c>
       <c r="C14" t="n">
-        <v>1290727.177071432</v>
+        <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>1.6990783870255583E10</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="n">
-        <v>130348.70106853993</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.1009885771246344</v>
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15">
@@ -2035,19 +2034,439 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
+        <v>1995.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F16" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1997.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1998.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2002.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F23" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2004.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F24" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2006.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2008.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2010.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2012.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2014.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="n">
         <v>2015.0</v>
       </c>
-      <c r="C15" t="n">
-        <v>1659129.0751294277</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1.795212894694677E10</v>
-      </c>
-      <c r="E15" t="n">
-        <v>133985.55499361403</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.08075655896944721</v>
+      <c r="C35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F35" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2016.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F36" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -2086,737 +2505,6 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1982.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F2" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1983.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1984.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1985.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1986.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F6" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1987.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F7" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1988.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F8" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1989.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F9" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1990.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F10" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1991.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F11" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1992.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F12" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1993.0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F13" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1994.0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1995.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1996.0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F16" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1997.0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F17" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1998.0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1999.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F19" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F20" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2001.0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F21" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="n">
-        <v>2002.0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F22" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2003.0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F23" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2004.0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F24" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" t="n">
-        <v>2005.0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F25" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2006.0</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F26" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="n">
-        <v>2007.0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F27" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="n">
-        <v>2008.0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F28" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="n">
-        <v>2009.0</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F29" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="n">
-        <v>2010.0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F30" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="n">
-        <v>2011.0</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F31" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" t="n">
-        <v>2012.0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F32" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2013.0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F33" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="n">
-        <v>2014.0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F34" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="n">
-        <v>2015.0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F35" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="n">
-        <v>2016.0</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F36" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="n">
         <v>1984.0</v>
       </c>
       <c r="C2" t="n">
@@ -4372,19 +4060,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1982.0</v>
+        <v>1980.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>146272.6377045942</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>8.907390934627414E8</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F2" t="e">
-        <v>#N/A</v>
+        <v>29845.252444278998</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.20403851952511556</v>
       </c>
     </row>
     <row r="3">
@@ -4395,16 +4083,16 @@
         <v>1983.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>215822.76010721733</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>9.600657119915833E8</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F3" t="e">
-        <v>#N/A</v>
+        <v>30984.927174217843</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.14356654116936055</v>
       </c>
     </row>
     <row r="4">
@@ -4412,19 +4100,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1984.0</v>
+        <v>1986.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>254697.33763241774</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>4.424261678090546E9</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="e">
-        <v>#N/A</v>
+        <v>66515.12367943508</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2611535884031521</v>
       </c>
     </row>
     <row r="5">
@@ -4432,19 +4120,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1985.0</v>
+        <v>1991.0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>188455.40641038126</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>6.512520704917269E8</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F5" t="e">
-        <v>#N/A</v>
+        <v>25519.640877013273</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.13541474539309103</v>
       </c>
     </row>
     <row r="6">
@@ -4452,19 +4140,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1986.0</v>
+        <v>1994.0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>184499.1323336066</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>1.1390395029914951E9</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F6" t="e">
-        <v>#N/A</v>
+        <v>33749.659301858075</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.18292584292934672</v>
       </c>
     </row>
     <row r="7">
@@ -4472,19 +4160,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1987.0</v>
+        <v>1997.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>83590.41205882984</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.1033975102517268E8</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F7" t="e">
-        <v>#N/A</v>
+        <v>10504.272988892315</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.12566361057652814</v>
       </c>
     </row>
     <row r="8">
@@ -4492,19 +4180,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>1988.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>136027.62366657282</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>5.56021471991911E8</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F8" t="e">
-        <v>#N/A</v>
+        <v>23580.10754835336</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.17334793413837968</v>
       </c>
     </row>
     <row r="9">
@@ -4512,19 +4200,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>1989.0</v>
+        <v>2002.0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>83152.53518582524</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>1.488715692716254E8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F9" t="e">
-        <v>#N/A</v>
+        <v>12201.293754009263</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.14673387560273904</v>
       </c>
     </row>
     <row r="10">
@@ -4532,19 +4220,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>1990.0</v>
+        <v>2004.0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0</v>
+        <v>114183.61308515805</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>3.9878993236840636E8</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F10" t="e">
-        <v>#N/A</v>
+        <v>19969.725395418096</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1748913426003142</v>
       </c>
     </row>
     <row r="11">
@@ -4552,19 +4240,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>1991.0</v>
+        <v>2006.0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0</v>
+        <v>92271.6827554874</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>5.979804512262157E8</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F11" t="e">
-        <v>#N/A</v>
+        <v>24453.63881360432</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2650178048492354</v>
       </c>
     </row>
     <row r="12">
@@ -4572,19 +4260,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>1992.0</v>
+        <v>2010.0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>68575.67328894761</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>1.199191169515322E8</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F12" t="e">
-        <v>#N/A</v>
+        <v>10950.758738623192</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1596886798687565</v>
       </c>
     </row>
     <row r="13">
@@ -4592,19 +4280,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>1993.0</v>
+        <v>2012.0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>65858.42897655317</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>8.142238892108728E7</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F13" t="e">
-        <v>#N/A</v>
+        <v>9023.435538700727</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.13701261446599702</v>
       </c>
     </row>
     <row r="14">
@@ -4612,19 +4300,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>1994.0</v>
+        <v>2014.0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
+        <v>86790.59850654732</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>1.965733549639212E8</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="e">
-        <v>#N/A</v>
+        <v>14020.4620096458</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.16154355714678154</v>
       </c>
     </row>
     <row r="15">
@@ -4632,439 +4320,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>1995.0</v>
+        <v>2016.0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>95734.84376933085</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>2.469083015430705E8</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1996.0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F16" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1997.0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F17" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1998.0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1999.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F19" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F20" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2001.0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F21" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="n">
-        <v>2002.0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F22" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2003.0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F23" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2004.0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F24" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" t="n">
-        <v>2005.0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F25" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2006.0</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F26" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="n">
-        <v>2007.0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F27" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="n">
-        <v>2008.0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F28" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="n">
-        <v>2009.0</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F29" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="n">
-        <v>2010.0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F30" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="n">
-        <v>2011.0</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F31" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" t="n">
-        <v>2012.0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F32" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2013.0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F33" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="n">
-        <v>2014.0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F34" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="n">
-        <v>2015.0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F35" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="n">
-        <v>2016.0</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F36" t="e">
-        <v>#N/A</v>
+        <v>15713.316058142233</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.16413372017405511</v>
       </c>
     </row>
   </sheetData>
@@ -5103,19 +4371,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1980.0</v>
+        <v>1984.0</v>
       </c>
       <c r="C2" t="n">
-        <v>146272.6377045942</v>
+        <v>39506.2652189262</v>
       </c>
       <c r="D2" t="n">
-        <v>8.907390934627414E8</v>
+        <v>1.2830973134799333E8</v>
       </c>
       <c r="E2" t="n">
-        <v>29845.252444278998</v>
+        <v>11327.388549352112</v>
       </c>
       <c r="F2" t="n">
-        <v>0.20403851952511556</v>
+        <v>0.28672385219358876</v>
       </c>
     </row>
     <row r="3">
@@ -5123,19 +4391,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1983.0</v>
+        <v>1987.0</v>
       </c>
       <c r="C3" t="n">
-        <v>215822.76010721733</v>
+        <v>136694.7292276805</v>
       </c>
       <c r="D3" t="n">
-        <v>9.600657119915833E8</v>
+        <v>1.5338936399278576E9</v>
       </c>
       <c r="E3" t="n">
-        <v>30984.927174217843</v>
+        <v>39164.95423114724</v>
       </c>
       <c r="F3" t="n">
-        <v>0.14356654116936055</v>
+        <v>0.28651400425186535</v>
       </c>
     </row>
     <row r="4">
@@ -5143,19 +4411,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1986.0</v>
+        <v>1990.0</v>
       </c>
       <c r="C4" t="n">
-        <v>254697.33763241774</v>
+        <v>107076.07709051284</v>
       </c>
       <c r="D4" t="n">
-        <v>4.424261678090546E9</v>
+        <v>2.0686461381030037E9</v>
       </c>
       <c r="E4" t="n">
-        <v>66515.12367943508</v>
+        <v>45482.37172908866</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2611535884031521</v>
+        <v>0.4247668850497932</v>
       </c>
     </row>
     <row r="5">
@@ -5163,19 +4431,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1991.0</v>
+        <v>1993.0</v>
       </c>
       <c r="C5" t="n">
-        <v>188455.40641038126</v>
+        <v>104479.59271794511</v>
       </c>
       <c r="D5" t="n">
-        <v>6.512520704917269E8</v>
+        <v>1.3523640469766798E9</v>
       </c>
       <c r="E5" t="n">
-        <v>25519.640877013273</v>
+        <v>36774.50267477019</v>
       </c>
       <c r="F5" t="n">
-        <v>0.13541474539309103</v>
+        <v>0.35197785249840385</v>
       </c>
     </row>
     <row r="6">
@@ -5183,19 +4451,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1994.0</v>
+        <v>1996.0</v>
       </c>
       <c r="C6" t="n">
-        <v>184499.1323336066</v>
+        <v>98965.05256508115</v>
       </c>
       <c r="D6" t="n">
-        <v>1.1390395029914951E9</v>
+        <v>7.073345677402056E8</v>
       </c>
       <c r="E6" t="n">
-        <v>33749.659301858075</v>
+        <v>26595.762213935617</v>
       </c>
       <c r="F6" t="n">
-        <v>0.18292584292934672</v>
+        <v>0.2687389287894914</v>
       </c>
     </row>
     <row r="7">
@@ -5203,19 +4471,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1997.0</v>
+        <v>1999.0</v>
       </c>
       <c r="C7" t="n">
-        <v>83590.41205882984</v>
+        <v>242186.97242413822</v>
       </c>
       <c r="D7" t="n">
-        <v>1.1033975102517268E8</v>
+        <v>2.164110293995178E10</v>
       </c>
       <c r="E7" t="n">
-        <v>10504.272988892315</v>
+        <v>147109.15314810217</v>
       </c>
       <c r="F7" t="n">
-        <v>0.12566361057652814</v>
+        <v>0.6074197619947626</v>
       </c>
     </row>
     <row r="8">
@@ -5223,19 +4491,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2000.0</v>
+        <v>2001.0</v>
       </c>
       <c r="C8" t="n">
-        <v>136027.62366657282</v>
+        <v>343613.6499993552</v>
       </c>
       <c r="D8" t="n">
-        <v>5.56021471991911E8</v>
+        <v>4.221983739068083E10</v>
       </c>
       <c r="E8" t="n">
-        <v>23580.10754835336</v>
+        <v>205474.66362225986</v>
       </c>
       <c r="F8" t="n">
-        <v>0.17334793413837968</v>
+        <v>0.5979816681399166</v>
       </c>
     </row>
     <row r="9">
@@ -5243,19 +4511,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2002.0</v>
+        <v>2003.0</v>
       </c>
       <c r="C9" t="n">
-        <v>83152.53518582524</v>
+        <v>66309.94663482861</v>
       </c>
       <c r="D9" t="n">
-        <v>1.488715692716254E8</v>
+        <v>1.021150676013936E9</v>
       </c>
       <c r="E9" t="n">
-        <v>12201.293754009263</v>
+        <v>31955.44829937355</v>
       </c>
       <c r="F9" t="n">
-        <v>0.14673387560273904</v>
+        <v>0.4819103305172815</v>
       </c>
     </row>
     <row r="10">
@@ -5263,19 +4531,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2004.0</v>
+        <v>2005.0</v>
       </c>
       <c r="C10" t="n">
-        <v>114183.61308515805</v>
+        <v>358998.6890254153</v>
       </c>
       <c r="D10" t="n">
-        <v>3.9878993236840636E8</v>
+        <v>1.753825308539476E10</v>
       </c>
       <c r="E10" t="n">
-        <v>19969.725395418096</v>
+        <v>132432.06970139357</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1748913426003142</v>
+        <v>0.36889290615771037</v>
       </c>
     </row>
     <row r="11">
@@ -5283,19 +4551,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2006.0</v>
+        <v>2007.0</v>
       </c>
       <c r="C11" t="n">
-        <v>92271.6827554874</v>
+        <v>221226.45728901695</v>
       </c>
       <c r="D11" t="n">
-        <v>5.979804512262157E8</v>
+        <v>7.153639777193719E9</v>
       </c>
       <c r="E11" t="n">
-        <v>24453.63881360432</v>
+        <v>84579.1923418149</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2650178048492354</v>
+        <v>0.3823195171964358</v>
       </c>
     </row>
     <row r="12">
@@ -5303,19 +4571,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2010.0</v>
+        <v>2009.0</v>
       </c>
       <c r="C12" t="n">
-        <v>68575.67328894761</v>
+        <v>89895.83939206997</v>
       </c>
       <c r="D12" t="n">
-        <v>1.199191169515322E8</v>
+        <v>8.344894648233004E8</v>
       </c>
       <c r="E12" t="n">
-        <v>10950.758738623192</v>
+        <v>28887.531303718224</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1596886798687565</v>
+        <v>0.32134447488419016</v>
       </c>
     </row>
     <row r="13">
@@ -5323,19 +4591,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2012.0</v>
+        <v>2011.0</v>
       </c>
       <c r="C13" t="n">
-        <v>65858.42897655317</v>
+        <v>173641.94723582527</v>
       </c>
       <c r="D13" t="n">
-        <v>8.142238892108728E7</v>
+        <v>4.504728200893002E9</v>
       </c>
       <c r="E13" t="n">
-        <v>9023.435538700727</v>
+        <v>67117.27200127402</v>
       </c>
       <c r="F13" t="n">
-        <v>0.13701261446599702</v>
+        <v>0.3865268333470208</v>
       </c>
     </row>
     <row r="14">
@@ -5343,19 +4611,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2014.0</v>
+        <v>2013.0</v>
       </c>
       <c r="C14" t="n">
-        <v>86790.59850654732</v>
+        <v>370454.0453848723</v>
       </c>
       <c r="D14" t="n">
-        <v>1.965733549639212E8</v>
+        <v>4.866998512803355E10</v>
       </c>
       <c r="E14" t="n">
-        <v>14020.4620096458</v>
+        <v>220612.74924181864</v>
       </c>
       <c r="F14" t="n">
-        <v>0.16154355714678154</v>
+        <v>0.5955198815891443</v>
       </c>
     </row>
     <row r="15">
@@ -5363,19 +4631,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2016.0</v>
+        <v>2015.0</v>
       </c>
       <c r="C15" t="n">
-        <v>95734.84376933085</v>
+        <v>48933.384995211214</v>
       </c>
       <c r="D15" t="n">
-        <v>2.469083015430705E8</v>
+        <v>2.7852858661167383E8</v>
       </c>
       <c r="E15" t="n">
-        <v>15713.316058142233</v>
+        <v>16689.17573194296</v>
       </c>
       <c r="F15" t="n">
-        <v>0.16413372017405511</v>
+        <v>0.3410590894861702</v>
       </c>
     </row>
   </sheetData>
@@ -5414,19 +4682,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1984.0</v>
+        <v>1980.0</v>
       </c>
       <c r="C2" t="n">
-        <v>39506.2652189262</v>
+        <v>37593.47178279423</v>
       </c>
       <c r="D2" t="n">
-        <v>1.2830973134799333E8</v>
+        <v>1.1469278344672582E9</v>
       </c>
       <c r="E2" t="n">
-        <v>11327.388549352112</v>
+        <v>33866.32301368511</v>
       </c>
       <c r="F2" t="n">
-        <v>0.28672385219358876</v>
+        <v>0.9008564893755049</v>
       </c>
     </row>
     <row r="3">
@@ -5434,19 +4702,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1987.0</v>
+        <v>1983.0</v>
       </c>
       <c r="C3" t="n">
-        <v>136694.7292276805</v>
+        <v>56367.90117042876</v>
       </c>
       <c r="D3" t="n">
-        <v>1.5338936399278576E9</v>
+        <v>7.531923204375198E7</v>
       </c>
       <c r="E3" t="n">
-        <v>39164.95423114724</v>
+        <v>8678.665337697495</v>
       </c>
       <c r="F3" t="n">
-        <v>0.28651400425186535</v>
+        <v>0.15396467062801375</v>
       </c>
     </row>
     <row r="4">
@@ -5454,19 +4722,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1990.0</v>
+        <v>1986.0</v>
       </c>
       <c r="C4" t="n">
-        <v>107076.07709051284</v>
+        <v>140405.03370105193</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0686461381030037E9</v>
+        <v>2.255266444371495E9</v>
       </c>
       <c r="E4" t="n">
-        <v>45482.37172908866</v>
+        <v>47489.645654305474</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4247668850497932</v>
+        <v>0.3382332128876493</v>
       </c>
     </row>
     <row r="5">
@@ -5474,19 +4742,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1993.0</v>
+        <v>1991.0</v>
       </c>
       <c r="C5" t="n">
-        <v>104479.59271794511</v>
+        <v>212812.83792393573</v>
       </c>
       <c r="D5" t="n">
-        <v>1.3523640469766798E9</v>
+        <v>1.0806767406439977E9</v>
       </c>
       <c r="E5" t="n">
-        <v>36774.50267477019</v>
+        <v>32873.64811888084</v>
       </c>
       <c r="F5" t="n">
-        <v>0.35197785249840385</v>
+        <v>0.15447211004549757</v>
       </c>
     </row>
     <row r="6">
@@ -5494,19 +4762,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1996.0</v>
+        <v>1994.0</v>
       </c>
       <c r="C6" t="n">
-        <v>98965.05256508115</v>
+        <v>88463.30021932717</v>
       </c>
       <c r="D6" t="n">
-        <v>7.073345677402056E8</v>
+        <v>1.9306058844496195E9</v>
       </c>
       <c r="E6" t="n">
-        <v>26595.762213935617</v>
+        <v>43938.66047627783</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2687389287894914</v>
+        <v>0.49668800923479745</v>
       </c>
     </row>
     <row r="7">
@@ -5514,19 +4782,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1999.0</v>
+        <v>1997.0</v>
       </c>
       <c r="C7" t="n">
-        <v>242186.97242413822</v>
+        <v>87391.37100469752</v>
       </c>
       <c r="D7" t="n">
-        <v>2.164110293995178E10</v>
+        <v>7.302366685706296E8</v>
       </c>
       <c r="E7" t="n">
-        <v>147109.15314810217</v>
+        <v>27022.89156568241</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6074197619947626</v>
+        <v>0.3092169313172791</v>
       </c>
     </row>
     <row r="8">
@@ -5534,19 +4802,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2001.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C8" t="n">
-        <v>343613.6499993552</v>
+        <v>205373.18662619212</v>
       </c>
       <c r="D8" t="n">
-        <v>4.221983739068083E10</v>
+        <v>3.627754487410157E9</v>
       </c>
       <c r="E8" t="n">
-        <v>205474.66362225986</v>
+        <v>60230.84332308619</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5979816681399166</v>
+        <v>0.2932751071965141</v>
       </c>
     </row>
     <row r="9">
@@ -5554,19 +4822,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2003.0</v>
+        <v>2002.0</v>
       </c>
       <c r="C9" t="n">
-        <v>66309.94663482861</v>
+        <v>178791.32853015303</v>
       </c>
       <c r="D9" t="n">
-        <v>1.021150676013936E9</v>
+        <v>2.2684949508626804E9</v>
       </c>
       <c r="E9" t="n">
-        <v>31955.44829937355</v>
+        <v>47628.719811293275</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4819103305172815</v>
+        <v>0.26639278427455015</v>
       </c>
     </row>
     <row r="10">
@@ -5574,19 +4842,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2005.0</v>
+        <v>2004.0</v>
       </c>
       <c r="C10" t="n">
-        <v>358998.6890254153</v>
+        <v>189446.11224836987</v>
       </c>
       <c r="D10" t="n">
-        <v>1.753825308539476E10</v>
+        <v>1.753885853889462E9</v>
       </c>
       <c r="E10" t="n">
-        <v>132432.06970139357</v>
+        <v>41879.42041014252</v>
       </c>
       <c r="F10" t="n">
-        <v>0.36889290615771037</v>
+        <v>0.22106244310380604</v>
       </c>
     </row>
     <row r="11">
@@ -5594,19 +4862,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2007.0</v>
+        <v>2006.0</v>
       </c>
       <c r="C11" t="n">
-        <v>221226.45728901695</v>
+        <v>219349.63424688563</v>
       </c>
       <c r="D11" t="n">
-        <v>7.153639777193719E9</v>
+        <v>2.833224663907719E9</v>
       </c>
       <c r="E11" t="n">
-        <v>84579.1923418149</v>
+        <v>53228.0439609396</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3823195171964358</v>
+        <v>0.24266301671161933</v>
       </c>
     </row>
     <row r="12">
@@ -5614,19 +4882,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2009.0</v>
+        <v>2010.0</v>
       </c>
       <c r="C12" t="n">
-        <v>89895.83939206997</v>
+        <v>217318.48485790766</v>
       </c>
       <c r="D12" t="n">
-        <v>8.344894648233004E8</v>
+        <v>2.2563857072257495E9</v>
       </c>
       <c r="E12" t="n">
-        <v>28887.531303718224</v>
+        <v>47501.42847563376</v>
       </c>
       <c r="F12" t="n">
-        <v>0.32134447488419016</v>
+        <v>0.21857978858398663</v>
       </c>
     </row>
     <row r="13">
@@ -5634,19 +4902,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2011.0</v>
+        <v>2012.0</v>
       </c>
       <c r="C13" t="n">
-        <v>173641.94723582527</v>
+        <v>285164.6025586077</v>
       </c>
       <c r="D13" t="n">
-        <v>4.504728200893002E9</v>
+        <v>2.060377673859271E10</v>
       </c>
       <c r="E13" t="n">
-        <v>67117.27200127402</v>
+        <v>143540.15723341223</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3865268333470208</v>
+        <v>0.5033589581088049</v>
       </c>
     </row>
     <row r="14">
@@ -5654,19 +4922,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2013.0</v>
+        <v>2014.0</v>
       </c>
       <c r="C14" t="n">
-        <v>370454.0453848723</v>
+        <v>472895.1507365388</v>
       </c>
       <c r="D14" t="n">
-        <v>4.866998512803355E10</v>
+        <v>2.1594362892526917E10</v>
       </c>
       <c r="E14" t="n">
-        <v>220612.74924181864</v>
+        <v>146950.20548650794</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5955198815891443</v>
+        <v>0.31074584980969155</v>
       </c>
     </row>
     <row r="15">
@@ -5674,19 +4942,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2015.0</v>
+        <v>2016.0</v>
       </c>
       <c r="C15" t="n">
-        <v>48933.384995211214</v>
+        <v>253216.46121030409</v>
       </c>
       <c r="D15" t="n">
-        <v>2.7852858661167383E8</v>
+        <v>2.177621011886313E9</v>
       </c>
       <c r="E15" t="n">
-        <v>16689.17573194296</v>
+        <v>46664.98700188732</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3410590894861702</v>
+        <v>0.18428891541585288</v>
       </c>
     </row>
   </sheetData>
@@ -5725,19 +4993,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1980.0</v>
+        <v>1984.0</v>
       </c>
       <c r="C2" t="n">
-        <v>37593.47178279423</v>
+        <v>68633.7891577465</v>
       </c>
       <c r="D2" t="n">
-        <v>1.1469278344672582E9</v>
+        <v>3.781212190838004E7</v>
       </c>
       <c r="E2" t="n">
-        <v>33866.32301368511</v>
+        <v>6149.156194827062</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9008564893755049</v>
+        <v>0.08959371572351872</v>
       </c>
     </row>
     <row r="3">
@@ -5745,19 +5013,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1983.0</v>
+        <v>1987.0</v>
       </c>
       <c r="C3" t="n">
-        <v>56367.90117042876</v>
+        <v>63394.41607893733</v>
       </c>
       <c r="D3" t="n">
-        <v>7.531923204375198E7</v>
+        <v>5.458865352012821E7</v>
       </c>
       <c r="E3" t="n">
-        <v>8678.665337697495</v>
+        <v>7388.413464345929</v>
       </c>
       <c r="F3" t="n">
-        <v>0.15396467062801375</v>
+        <v>0.11654675476695045</v>
       </c>
     </row>
     <row r="4">
@@ -5765,19 +5033,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1986.0</v>
+        <v>1990.0</v>
       </c>
       <c r="C4" t="n">
-        <v>140405.03370105193</v>
+        <v>96596.8190505549</v>
       </c>
       <c r="D4" t="n">
-        <v>2.255266444371495E9</v>
+        <v>1.5313196731019202E8</v>
       </c>
       <c r="E4" t="n">
-        <v>47489.645654305474</v>
+        <v>12374.650189407055</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3382332128876493</v>
+        <v>0.12810618725375067</v>
       </c>
     </row>
     <row r="5">
@@ -5785,19 +5053,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>1991.0</v>
+        <v>1993.0</v>
       </c>
       <c r="C5" t="n">
-        <v>212812.83792393573</v>
+        <v>85549.05085398392</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0806767406439977E9</v>
+        <v>4.148786820351742E7</v>
       </c>
       <c r="E5" t="n">
-        <v>32873.64811888084</v>
+        <v>6441.107684514941</v>
       </c>
       <c r="F5" t="n">
-        <v>0.15447211004549757</v>
+        <v>0.0752913985627812</v>
       </c>
     </row>
     <row r="6">
@@ -5805,19 +5073,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1994.0</v>
+        <v>1996.0</v>
       </c>
       <c r="C6" t="n">
-        <v>88463.30021932717</v>
+        <v>79530.24950163432</v>
       </c>
       <c r="D6" t="n">
-        <v>1.9306058844496195E9</v>
+        <v>3.1628340545021616E7</v>
       </c>
       <c r="E6" t="n">
-        <v>43938.66047627783</v>
+        <v>5623.907942438391</v>
       </c>
       <c r="F6" t="n">
-        <v>0.49668800923479745</v>
+        <v>0.07071407392381966</v>
       </c>
     </row>
     <row r="7">
@@ -5825,19 +5093,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>1997.0</v>
+        <v>1999.0</v>
       </c>
       <c r="C7" t="n">
-        <v>87391.37100469752</v>
+        <v>74245.21680594703</v>
       </c>
       <c r="D7" t="n">
-        <v>7.302366685706296E8</v>
+        <v>2.7413205957390133E7</v>
       </c>
       <c r="E7" t="n">
-        <v>27022.89156568241</v>
+        <v>5235.762213602728</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3092169313172791</v>
+        <v>0.07051985890602644</v>
       </c>
     </row>
     <row r="8">
@@ -5845,19 +5113,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>2000.0</v>
+        <v>2001.0</v>
       </c>
       <c r="C8" t="n">
-        <v>205373.18662619212</v>
+        <v>32423.90797904045</v>
       </c>
       <c r="D8" t="n">
-        <v>3.627754487410157E9</v>
+        <v>1.4122295718716972E7</v>
       </c>
       <c r="E8" t="n">
-        <v>60230.84332308619</v>
+        <v>3757.9643051414114</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2932751071965141</v>
+        <v>0.11590102919027048</v>
       </c>
     </row>
     <row r="9">
@@ -5865,19 +5133,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>2002.0</v>
+        <v>2003.0</v>
       </c>
       <c r="C9" t="n">
-        <v>178791.32853015303</v>
+        <v>99296.62617433087</v>
       </c>
       <c r="D9" t="n">
-        <v>2.2684949508626804E9</v>
+        <v>1.1118576120922644E8</v>
       </c>
       <c r="E9" t="n">
-        <v>47628.719811293275</v>
+        <v>10544.46590440817</v>
       </c>
       <c r="F9" t="n">
-        <v>0.26639278427455015</v>
+        <v>0.10619158284286215</v>
       </c>
     </row>
     <row r="10">
@@ -5885,19 +5153,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2004.0</v>
+        <v>2005.0</v>
       </c>
       <c r="C10" t="n">
-        <v>189446.11224836987</v>
+        <v>80560.47717498823</v>
       </c>
       <c r="D10" t="n">
-        <v>1.753885853889462E9</v>
+        <v>4.620545637460832E7</v>
       </c>
       <c r="E10" t="n">
-        <v>41879.42041014252</v>
+        <v>6797.459552995392</v>
       </c>
       <c r="F10" t="n">
-        <v>0.22106244310380604</v>
+        <v>0.08437710141947635</v>
       </c>
     </row>
     <row r="11">
@@ -5905,19 +5173,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>2006.0</v>
+        <v>2007.0</v>
       </c>
       <c r="C11" t="n">
-        <v>219349.63424688563</v>
+        <v>71468.5091960996</v>
       </c>
       <c r="D11" t="n">
-        <v>2.833224663907719E9</v>
+        <v>5.056779960558433E7</v>
       </c>
       <c r="E11" t="n">
-        <v>53228.0439609396</v>
+        <v>7111.103965319613</v>
       </c>
       <c r="F11" t="n">
-        <v>0.24266301671161933</v>
+        <v>0.09949982230366296</v>
       </c>
     </row>
     <row r="12">
@@ -5925,19 +5193,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>2010.0</v>
+        <v>2009.0</v>
       </c>
       <c r="C12" t="n">
-        <v>217318.48485790766</v>
+        <v>76276.93110273265</v>
       </c>
       <c r="D12" t="n">
-        <v>2.2563857072257495E9</v>
+        <v>4.1433952986025654E7</v>
       </c>
       <c r="E12" t="n">
-        <v>47501.42847563376</v>
+        <v>6436.9210796797615</v>
       </c>
       <c r="F12" t="n">
-        <v>0.21857978858398663</v>
+        <v>0.08438883141496967</v>
       </c>
     </row>
     <row r="13">
@@ -5945,19 +5213,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>2012.0</v>
+        <v>2011.0</v>
       </c>
       <c r="C13" t="n">
-        <v>285164.6025586077</v>
+        <v>77530.87007075697</v>
       </c>
       <c r="D13" t="n">
-        <v>2.060377673859271E10</v>
+        <v>5.472765854450502E7</v>
       </c>
       <c r="E13" t="n">
-        <v>143540.15723341223</v>
+        <v>7397.814443773582</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5033589581088049</v>
+        <v>0.09541766314530092</v>
       </c>
     </row>
     <row r="14">
@@ -5965,19 +5233,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>2014.0</v>
+        <v>2013.0</v>
       </c>
       <c r="C14" t="n">
-        <v>472895.1507365388</v>
+        <v>82738.89311549942</v>
       </c>
       <c r="D14" t="n">
-        <v>2.1594362892526917E10</v>
+        <v>3.200149172776994E8</v>
       </c>
       <c r="E14" t="n">
-        <v>146950.20548650794</v>
+        <v>17888.960765726428</v>
       </c>
       <c r="F14" t="n">
-        <v>0.31074584980969155</v>
+        <v>0.21620981490233765</v>
       </c>
     </row>
     <row r="15">
@@ -5985,19 +5253,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2016.0</v>
+        <v>2015.0</v>
       </c>
       <c r="C15" t="n">
-        <v>253216.46121030409</v>
+        <v>53067.00075185715</v>
       </c>
       <c r="D15" t="n">
-        <v>2.177621011886313E9</v>
+        <v>2.4956950153002646E7</v>
       </c>
       <c r="E15" t="n">
-        <v>46664.98700188732</v>
+        <v>4995.693160413542</v>
       </c>
       <c r="F15" t="n">
-        <v>0.18428891541585288</v>
+        <v>0.09413935382882385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>